<commit_message>
Update my client program (activity_01_main.py) by testing my solution
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ADD\Term2\intermediate_software_development\activities\activity_1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05B8C71-4829-4298-ABBF-A03C0D7921DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B47481C-9292-43BD-8221-A1CE5D3C64A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="0" windowWidth="16200" windowHeight="9428" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>raise valueError  when the value of is_borrowed is invalid</t>
+  </si>
+  <si>
+    <t>self.__is_borrowed = " "</t>
   </si>
 </sst>
 </file>
@@ -1226,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1529,13 +1532,13 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" ht="58.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="12">
         <v>14</v>
       </c>
@@ -1554,8 +1557,8 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="12">
-        <v>14</v>
+      <c r="B21" s="11">
+        <v>15</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1564,8 +1567,8 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="11">
-        <v>15</v>
+      <c r="B22" s="12">
+        <v>16</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1575,7 +1578,7 @@
     </row>
     <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1585,7 +1588,7 @@
     </row>
     <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1595,7 +1598,7 @@
     </row>
     <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="11">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1604,8 +1607,8 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="11">
-        <v>19</v>
+      <c r="B26" s="12">
+        <v>20</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1614,8 +1617,8 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="12">
-        <v>20</v>
+      <c r="B27" s="11">
+        <v>21</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>

</xml_diff>